<commit_message>
Sección de implementation and results del paper
</commit_message>
<xml_diff>
--- a/Notes/Metricas Occlusion.xlsx
+++ b/Notes/Metricas Occlusion.xlsx
@@ -400,11 +400,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43189376"/>
-        <c:axId val="43190912"/>
+        <c:axId val="77372800"/>
+        <c:axId val="79180928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43189376"/>
+        <c:axId val="77372800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,7 +414,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43190912"/>
+        <c:crossAx val="79180928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -422,7 +422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43190912"/>
+        <c:axId val="79180928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
@@ -440,7 +440,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>FPS</a:t>
                 </a:r>
               </a:p>
@@ -453,7 +453,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43189376"/>
+        <c:crossAx val="77372800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -501,14 +501,9 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Culling</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Discarded objects</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> %</a:t>
-            </a:r>
-            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -785,11 +780,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43263872"/>
-        <c:axId val="74078464"/>
+        <c:axId val="79227136"/>
+        <c:axId val="79040512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43263872"/>
+        <c:axId val="79227136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,7 +794,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74078464"/>
+        <c:crossAx val="79040512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -807,7 +802,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74078464"/>
+        <c:axId val="79040512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,8 +819,8 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="es-ES"/>
-                  <a:t>FPS</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% discarded objects</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -837,7 +832,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43263872"/>
+        <c:crossAx val="79227136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2"/>
@@ -1238,7 +1233,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
# Haciendo papers en latex
</commit_message>
<xml_diff>
--- a/Notes/Metricas Occlusion.xlsx
+++ b/Notes/Metricas Occlusion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -48,8 +48,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,38 +99,24 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="129"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="29"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>Occlusion Culling</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>performance</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -245,6 +231,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -360,17 +347,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="84849408"/>
-        <c:axId val="84850944"/>
+        <c:smooth val="0"/>
+        <c:axId val="76681600"/>
+        <c:axId val="76683520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84849408"/>
+        <c:axId val="76681600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -383,33 +380,32 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-AR"/>
-                  <a:t>Selected</a:t>
+                  <a:t>Selected View Points</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="es-AR" baseline="0"/>
-                  <a:t> View Points</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84850944"/>
+        <c:crossAx val="76683520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84850944"/>
+        <c:axId val="76683520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -429,11 +425,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84849408"/>
+        <c:crossAx val="76681600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5"/>
@@ -443,9 +441,11 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -457,30 +457,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="126"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="26"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Percentage of discarded objects</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -595,6 +589,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -710,17 +705,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="84905984"/>
-        <c:axId val="84907520"/>
+        <c:smooth val="0"/>
+        <c:axId val="76738944"/>
+        <c:axId val="76740864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84905984"/>
+        <c:axId val="76738944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -733,32 +738,31 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-AR"/>
-                  <a:t>Selected View</a:t>
+                  <a:t>Selected View Points</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="es-AR" baseline="0"/>
-                  <a:t> Points</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84907520"/>
+        <c:crossAx val="76740864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84907520"/>
+        <c:axId val="76740864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -772,17 +776,19 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>% Discarded Objects</a:t>
+                  <a:t>% discarded objects</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84905984"/>
+        <c:crossAx val="76738944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="2"/>
@@ -791,10 +797,19 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </a:scene3d>
+    <a:sp3d/>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
@@ -966,6 +981,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1000,6 +1016,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1175,14 +1192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
@@ -1194,14 +1211,14 @@
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1227,7 +1244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1255,7 +1272,7 @@
         <v>93.80952380952381</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1283,7 +1300,7 @@
         <v>82.38095238095238</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1311,7 +1328,7 @@
         <v>81.904761904761898</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1339,7 +1356,7 @@
         <v>91.428571428571431</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1367,7 +1384,7 @@
         <v>86.666666666666671</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1395,7 +1412,7 @@
         <v>79.523809523809518</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1423,7 +1440,7 @@
         <v>92.857142857142861</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1451,7 +1468,7 @@
         <v>86.666666666666671</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1479,7 +1496,7 @@
         <v>90.952380952380949</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1507,7 +1524,7 @@
         <v>85.238095238095241</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1535,7 +1552,7 @@
         <v>83.80952380952381</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1563,7 +1580,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1591,7 +1608,7 @@
         <v>93.80952380952381</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1619,7 +1636,7 @@
         <v>87.61904761904762</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1660,24 +1677,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>